<commit_message>
Commiting some minor changes to CNV samples collected. As well as changed to CNVkit post processing script. And more importantly script to change file names on system in order to remove value coming after MolDx number based on a GT list
</commit_message>
<xml_diff>
--- a/CNVkit_tests/CollectingCNVSamples/CNVSamples.xlsx
+++ b/CNVkit_tests/CollectingCNVSamples/CNVSamples.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/HAEMATONC/SHARED/Diagnostics/MOLECULAR DIAGNOSTICS/TRANSLATIONAL RESEARCH/9999_Data4Debbie/Sabri/CNVkit_tests/CollectingCNVSamples/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sjamal/Documents/Work/2.Scripts/geneCN/CNVkit_tests/CollectingCNVSamples/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="1440" windowWidth="40980" windowHeight="24260" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="6280" yWindow="3040" windowWidth="40980" windowHeight="24260" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="SamplesValidationData" sheetId="2" r:id="rId2"/>
     <sheet name="PAEDSamplesMissingData" sheetId="3" r:id="rId3"/>
-    <sheet name="RMH200 CNA alterations" sheetId="4" r:id="rId4"/>
+    <sheet name="RMH200 CNA run1" sheetId="6" r:id="rId4"/>
+    <sheet name="RMH200 CAN run2" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1336" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1383" uniqueCount="408">
   <si>
     <t xml:space="preserve">Negatives </t>
   </si>
@@ -1146,13 +1147,121 @@
   </si>
   <si>
     <t>L210</t>
+  </si>
+  <si>
+    <t>Diagnosis</t>
+  </si>
+  <si>
+    <t>Mdx number</t>
+  </si>
+  <si>
+    <t>Secondary ID</t>
+  </si>
+  <si>
+    <t>Path number</t>
+  </si>
+  <si>
+    <t>MDS case with Hyperdiploid karyotype</t>
+  </si>
+  <si>
+    <t>18/02561</t>
+  </si>
+  <si>
+    <t>smith</t>
+  </si>
+  <si>
+    <t>51,XX,+10,+12,+13,+19,+21[10]</t>
+  </si>
+  <si>
+    <t>ALL Cases with Hyperdiploid karyotype</t>
+  </si>
+  <si>
+    <t>18/06274</t>
+  </si>
+  <si>
+    <t>GUSCIORA</t>
+  </si>
+  <si>
+    <t>46,XX[11] low mitotic index and normal karyotype</t>
+  </si>
+  <si>
+    <t>FISH found gains of chromosomes +6, +10, +14, +14, +17, +18, +21, +21</t>
+  </si>
+  <si>
+    <t>18/06260</t>
+  </si>
+  <si>
+    <t>IGLESIAS-GARCIA</t>
+  </si>
+  <si>
+    <t>54,XY,+X,+4,+6,+8,+14,+17,+21,+21[9]/46,XY[1]</t>
+  </si>
+  <si>
+    <t>Myeloid cases with +8</t>
+  </si>
+  <si>
+    <t>18/08101</t>
+  </si>
+  <si>
+    <t>DEVANI</t>
+  </si>
+  <si>
+    <t>47,XY,+8[3]/46,XY[10] - 23% of cells have +8</t>
+  </si>
+  <si>
+    <t>18/03379</t>
+  </si>
+  <si>
+    <t>EDMONDS</t>
+  </si>
+  <si>
+    <t>+8 in 100% of cells</t>
+  </si>
+  <si>
+    <t>18/06405</t>
+  </si>
+  <si>
+    <t>WILSON</t>
+  </si>
+  <si>
+    <t>+8 in 50% of cells</t>
+  </si>
+  <si>
+    <t>17/13252</t>
+  </si>
+  <si>
+    <t>FARRUGIA</t>
+  </si>
+  <si>
+    <t>+8 in 17% of cells</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>WHITAKER</t>
+  </si>
+  <si>
+    <t>47,XX,+8[2]/51~53,XX,+X,+4,+6,+8,+8,+8,+10,+?18[cp5]/46,XX[15] - cp means composite karyotype ie some variation (see page 92 of ICSN for explanation)</t>
+  </si>
+  <si>
+    <t>HARFLEET</t>
+  </si>
+  <si>
+    <t>53~54,XY,+X,+5,der(8)t(1;8)(q11;q24),t(9;22)(q34;q11.2),+14,+16,+18,+18,+21,+mar[cp8]/46,XY[2] Also Ph+ve</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STOFFELL </t>
+  </si>
+  <si>
+    <t>47,XY,+8[12] - All cells have +8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1185,6 +1294,13 @@
       <sz val="15"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1262,7 +1378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1296,8 +1412,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1305,8 +1458,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1342,14 +1497,27 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1934,8 +2102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG107"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="X11" sqref="X11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5561,13 +5729,14 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="I1" sqref="I1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="48.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -6356,10 +6525,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6385,58 +6554,55 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
-        <v>356</v>
+      <c r="A2" s="26" t="s">
+        <v>359</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>361</v>
+        <v>368</v>
+      </c>
+      <c r="D3" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="20" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
-        <v>362</v>
+        <v>370</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>363</v>
+        <v>38</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>364</v>
-      </c>
-      <c r="D4" s="25" t="s">
-        <v>365</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>366</v>
+      <c r="A5" s="25" t="s">
+        <v>371</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>367</v>
+        <v>38</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>368</v>
-      </c>
-      <c r="D5" t="s">
-        <v>369</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
-        <v>370</v>
+      <c r="A6" s="25">
+        <v>644060</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>38</v>
@@ -6446,8 +6612,8 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>371</v>
+      <c r="A7" s="25">
+        <v>2027047</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>38</v>
@@ -6456,26 +6622,262 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
-        <v>644060</v>
-      </c>
-      <c r="B8" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="20" x14ac:dyDescent="0.25">
-      <c r="A9" s="25">
-        <v>2027047</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>38</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="116" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="27" t="s">
+        <v>372</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1" s="28" t="s">
+        <v>374</v>
+      </c>
+      <c r="D1" s="28" t="s">
+        <v>375</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>376</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>377</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>378</v>
+      </c>
+      <c r="D2" s="31">
+        <v>2042496</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>379</v>
+      </c>
+      <c r="F2" s="30"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
+        <v>380</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>381</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>382</v>
+      </c>
+      <c r="D3" s="31">
+        <v>2047387</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>383</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
+        <v>380</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>385</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>386</v>
+      </c>
+      <c r="D4" s="31">
+        <v>2047368</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>387</v>
+      </c>
+      <c r="F4" s="30"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>389</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>390</v>
+      </c>
+      <c r="D5" s="31">
+        <v>2049738</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>391</v>
+      </c>
+      <c r="F5" s="30"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>392</v>
+      </c>
+      <c r="C6" s="30" t="s">
+        <v>393</v>
+      </c>
+      <c r="D6" s="31">
+        <v>2043708</v>
+      </c>
+      <c r="E6" s="30" t="s">
+        <v>394</v>
+      </c>
+      <c r="F6" s="30"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>395</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>396</v>
+      </c>
+      <c r="D7" s="31">
+        <v>2047546</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>397</v>
+      </c>
+      <c r="F7" s="30"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="C8" s="30" t="s">
+        <v>399</v>
+      </c>
+      <c r="D8" s="31">
+        <v>2038382</v>
+      </c>
+      <c r="E8" s="30" t="s">
+        <v>400</v>
+      </c>
+      <c r="F8" s="30"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>401</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>402</v>
+      </c>
+      <c r="D10" s="28">
+        <v>2039557</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>403</v>
+      </c>
+      <c r="F10" s="33"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
+        <v>380</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>401</v>
+      </c>
+      <c r="C11" s="30" t="s">
+        <v>404</v>
+      </c>
+      <c r="D11" s="30">
+        <v>2034598</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>405</v>
+      </c>
+      <c r="F11" s="31"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
+        <v>388</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>401</v>
+      </c>
+      <c r="C12" s="30" t="s">
+        <v>406</v>
+      </c>
+      <c r="D12" s="30">
+        <v>2051478</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>407</v>
+      </c>
+      <c r="F12" s="30"/>
+    </row>
+    <row r="14" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+      <c r="C14" s="25" t="s">
+        <v>356</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>357</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="20" x14ac:dyDescent="0.25">
+      <c r="C15" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>

</xml_diff>